<commit_message>
Update scripts to output nr of studies and effect sizes for each moderator level.
</commit_message>
<xml_diff>
--- a/output/02-overall-design.xlsx
+++ b/output/02-overall-design.xlsx
@@ -10,6 +10,7 @@
     <sheet name="descriptives" sheetId="1" r:id="rId1"/>
     <sheet name="coefficients" sheetId="2" r:id="rId2"/>
     <sheet name="pairwise" sheetId="3" r:id="rId3"/>
+    <sheet name="nr_studies" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -411,22 +412,22 @@
         <v>82</v>
       </c>
       <c r="C2">
-        <v>742</v>
+        <v>845</v>
       </c>
       <c r="D2">
-        <v>0.009103327877982365</v>
+        <v>0.008095743408439994</v>
       </c>
       <c r="E2">
-        <v>0.05348101551452059</v>
+        <v>0.05052704415099526</v>
       </c>
       <c r="F2">
-        <v>96.97324000486512</v>
+        <v>97.73316103332681</v>
       </c>
       <c r="G2">
-        <v>82.86780801817574</v>
+        <v>84.23631744806789</v>
       </c>
       <c r="H2">
-        <v>14.10543198668938</v>
+        <v>13.49684358525892</v>
       </c>
     </row>
     <row r="3">
@@ -439,22 +440,22 @@
         <v>51</v>
       </c>
       <c r="C3">
-        <v>385</v>
+        <v>438</v>
       </c>
       <c r="D3">
-        <v>0.004324793876700262</v>
+        <v>0.002763808288530445</v>
       </c>
       <c r="E3">
-        <v>0.05650692452892183</v>
+        <v>0.05318914704310809</v>
       </c>
       <c r="F3">
-        <v>95.16775494513507</v>
+        <v>95.02046485971272</v>
       </c>
       <c r="G3">
-        <v>88.40186151595992</v>
+        <v>90.32690851755481</v>
       </c>
       <c r="H3">
-        <v>6.765893429175146</v>
+        <v>4.693556342157903</v>
       </c>
     </row>
   </sheetData>
@@ -539,22 +540,22 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.1509031501759658</v>
+        <v>-0.1597154571624137</v>
       </c>
       <c r="E2">
-        <v>4.83366714489929e-17</v>
+        <v>2.269635605788456e-14</v>
       </c>
       <c r="F2">
-        <v>3145944859403054</v>
+        <v>-7097821819688.762</v>
       </c>
       <c r="G2">
-        <v>2.023620250255691e-16</v>
+        <v>8.969227300150751e-14</v>
       </c>
       <c r="H2">
-        <v>0.1509031501759652</v>
+        <v>-0.1597154571626948</v>
       </c>
       <c r="I2">
-        <v>0.1509031501759664</v>
+        <v>-0.1597154571621327</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -577,25 +578,25 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.1309228341860756</v>
+        <v>0.1213364039631816</v>
       </c>
       <c r="E3">
-        <v>0.01914799361926669</v>
+        <v>0.01855766108550308</v>
       </c>
       <c r="F3">
-        <v>6.876890898983978</v>
+        <v>6.570719159327477</v>
       </c>
       <c r="G3">
-        <v>5.540443431896286e-09</v>
+        <v>1.774098066587662e-08</v>
       </c>
       <c r="H3">
-        <v>0.0930502262048588</v>
+        <v>0.08455854362394009</v>
       </c>
       <c r="I3">
-        <v>0.1684171350136906</v>
+        <v>0.1577841082989081</v>
       </c>
       <c r="J3">
-        <v>55.97098003600755</v>
+        <v>55.94756359842736</v>
       </c>
     </row>
     <row r="4">
@@ -615,22 +616,22 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.003974339101933848</v>
+        <v>0.003972252781116893</v>
       </c>
       <c r="E4">
-        <v>5.94910929937305e-05</v>
+        <v>6.293566203749799e-05</v>
       </c>
       <c r="F4">
-        <v>66.80596754102775</v>
+        <v>63.11641993053626</v>
       </c>
       <c r="G4">
-        <v>0.009528673180206868</v>
+        <v>0.01008559281622121</v>
       </c>
       <c r="H4">
-        <v>0.003218442907280631</v>
+        <v>0.003172589622263816</v>
       </c>
       <c r="I4">
-        <v>0.004730230754834357</v>
+        <v>0.004771910859719281</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -653,25 +654,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.09013426256400539</v>
+        <v>0.1229849656393078</v>
       </c>
       <c r="E5">
-        <v>0.01188430504611599</v>
+        <v>0.06178650348428123</v>
       </c>
       <c r="F5">
-        <v>7.604950237051677</v>
+        <v>2.000610310205984</v>
       </c>
       <c r="G5">
-        <v>0.08323370938287843</v>
+        <v>0.2950895471579177</v>
       </c>
       <c r="H5">
-        <v>-0.06055070059452931</v>
+        <v>-0.5793350450826276</v>
       </c>
       <c r="I5">
-        <v>0.2368025322597377</v>
+        <v>0.7204993810036464</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0.9999999999999982</v>
       </c>
     </row>
     <row r="6">
@@ -691,22 +692,22 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.05472045850693689</v>
+        <v>0.0480027512630412</v>
       </c>
       <c r="E6">
-        <v>0.2435102734470063</v>
+        <v>0.236169282017018</v>
       </c>
       <c r="F6">
-        <v>0.2249398888910043</v>
+        <v>0.2034120282344944</v>
       </c>
       <c r="G6">
-        <v>0.859143274517422</v>
+        <v>0.8722468408253656</v>
       </c>
       <c r="H6">
-        <v>-0.9954278601185784</v>
+        <v>-0.994566243336082</v>
       </c>
       <c r="I6">
-        <v>0.9963258178940084</v>
+        <v>0.9955140641870832</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -729,25 +730,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.06891890101067315</v>
+        <v>0.03454035753874145</v>
       </c>
       <c r="E7">
-        <v>0.03827401673706031</v>
+        <v>0.0205491837863112</v>
       </c>
       <c r="F7">
-        <v>1.803529816520294</v>
+        <v>1.681531670830845</v>
       </c>
       <c r="G7">
-        <v>0.1041590482135323</v>
+        <v>0.1250473182328547</v>
       </c>
       <c r="H7">
-        <v>-0.01729734360638192</v>
+        <v>-0.01153354948722172</v>
       </c>
       <c r="I7">
-        <v>0.1541178216815295</v>
+        <v>0.08046791089556368</v>
       </c>
       <c r="J7">
-        <v>9.177393280147998</v>
+        <v>9.538981409281005</v>
       </c>
     </row>
     <row r="8">
@@ -767,22 +768,22 @@
         </is>
       </c>
       <c r="D8">
-        <v>-0.1200487213609953</v>
+        <v>0.04491997566670915</v>
       </c>
       <c r="E8">
-        <v>5.541913677481827e-17</v>
+        <v>2.221481368528577e-15</v>
       </c>
       <c r="F8">
-        <v>-2176693267362433</v>
+        <v>20234347302518.88</v>
       </c>
       <c r="G8">
-        <v>2.924710531856393e-16</v>
+        <v>3.146233297519468e-14</v>
       </c>
       <c r="H8">
-        <v>-0.120048721360996</v>
+        <v>0.04491997566668098</v>
       </c>
       <c r="I8">
-        <v>-0.1200487213609946</v>
+        <v>0.04491997566673731</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -805,25 +806,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.04540884667313749</v>
+        <v>0.03775206423673266</v>
       </c>
       <c r="E9">
-        <v>0.02035422312622509</v>
+        <v>0.01870525575479194</v>
       </c>
       <c r="F9">
-        <v>2.23246524912769</v>
+        <v>2.01921936072586</v>
       </c>
       <c r="G9">
-        <v>0.03197961455437517</v>
+        <v>0.05102290451872862</v>
       </c>
       <c r="H9">
-        <v>0.004141215989380611</v>
+        <v>-0.0001772413081629961</v>
       </c>
       <c r="I9">
-        <v>0.08652207355452135</v>
+        <v>0.07557290314991361</v>
       </c>
       <c r="J9">
-        <v>35.53955441607282</v>
+        <v>35.69552461908427</v>
       </c>
     </row>
     <row r="10">
@@ -843,25 +844,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.1808820452475528</v>
+        <v>0.1849994946729422</v>
       </c>
       <c r="E10">
-        <v>0.0929261834011034</v>
+        <v>0.08723663062783917</v>
       </c>
       <c r="F10">
-        <v>1.968168843424003</v>
+        <v>2.145365376706126</v>
       </c>
       <c r="G10">
-        <v>0.2992723156408777</v>
+        <v>0.2776801997575834</v>
       </c>
       <c r="H10">
-        <v>-0.7606874953554431</v>
+        <v>-0.7265080720437419</v>
       </c>
       <c r="I10">
-        <v>0.8772331322767427</v>
+        <v>0.8605863923566883</v>
       </c>
       <c r="J10">
-        <v>1.000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -881,25 +882,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.1225509200257808</v>
+        <v>0.1091262032705729</v>
       </c>
       <c r="E11">
-        <v>0.07071931490959343</v>
+        <v>0.04309853415595803</v>
       </c>
       <c r="F11">
-        <v>1.741674511535374</v>
+        <v>2.542139879805543</v>
       </c>
       <c r="G11">
-        <v>0.1446090684273876</v>
+        <v>0.05881625065882558</v>
       </c>
       <c r="H11">
-        <v>-0.06097352177482309</v>
+        <v>-0.006307984203805485</v>
       </c>
       <c r="I11">
-        <v>0.2980601947104344</v>
+        <v>0.2216902961138924</v>
       </c>
       <c r="J11">
-        <v>4.789509791339099</v>
+        <v>4.359205059832483</v>
       </c>
     </row>
   </sheetData>
@@ -964,19 +965,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>1.064646271396447</v>
+        <v>15.25148396653277</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>55.97098003600753</v>
+        <v>55.94756359842755</v>
       </c>
       <c r="F2">
-        <v>0.291607500841684</v>
+        <v>1.384407059621348e-21</v>
       </c>
       <c r="G2">
-        <v>0.5175540106298814</v>
+        <v>2.076610589432022e-20</v>
       </c>
     </row>
     <row r="3">
@@ -991,7 +992,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>2489.282606619797</v>
+        <v>2622.789044953463</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1000,10 +1001,10 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.0002557442599842066</v>
+        <v>0.0002427262469866367</v>
       </c>
       <c r="G3">
-        <v>0.00191808194988155</v>
+        <v>0.0009102234261998876</v>
       </c>
     </row>
     <row r="4">
@@ -1018,19 +1019,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>5.190455339929126</v>
+        <v>4.607889929064195</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.9999999999999984</v>
       </c>
       <c r="F4">
-        <v>0.1211673866826639</v>
+        <v>0.1360489697985592</v>
       </c>
       <c r="G4">
-        <v>0.3068871524944256</v>
+        <v>0.3401224244963979</v>
       </c>
     </row>
     <row r="5">
@@ -1045,7 +1046,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.3995286434344152</v>
+        <v>0.88552737312287</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1054,10 +1055,10 @@
         <v>0.9999999999999996</v>
       </c>
       <c r="F5">
-        <v>0.7580208441235643</v>
+        <v>0.53860256822631</v>
       </c>
       <c r="G5">
-        <v>0.9600094535782364</v>
+        <v>0.807903852339465</v>
       </c>
     </row>
     <row r="6">
@@ -1072,19 +1073,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>2.16951811597881</v>
+        <v>9.521000767525148</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>9.177393280147989</v>
+        <v>9.538981409280998</v>
       </c>
       <c r="F6">
-        <v>0.05758849816288313</v>
+        <v>3.527848647479622e-06</v>
       </c>
       <c r="G6">
-        <v>0.2879424908144156</v>
+        <v>1.763924323739811e-05</v>
       </c>
     </row>
     <row r="7">
@@ -1099,19 +1100,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>6.669298580964861</v>
+        <v>6.356632264173754</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>55.98318819311954</v>
+        <v>55.96196981240531</v>
       </c>
       <c r="F7">
-        <v>1.21765415174255e-08</v>
+        <v>3.983221008873925e-08</v>
       </c>
       <c r="G7">
-        <v>1.826481227613825e-07</v>
+        <v>2.987415756655444e-07</v>
       </c>
     </row>
     <row r="8">
@@ -1126,19 +1127,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>1.83256409679453</v>
+        <v>0.02594097773135135</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1.040713778963249</v>
+        <v>1.040428343873796</v>
       </c>
       <c r="F8">
-        <v>0.3105324063779288</v>
+        <v>0.98336390185164</v>
       </c>
       <c r="G8">
-        <v>0.5175540106298814</v>
+        <v>0.98336390185164</v>
       </c>
     </row>
     <row r="9">
@@ -1153,19 +1154,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.3148402361833432</v>
+        <v>0.3119390382671925</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1.076233336486658</v>
+        <v>1.074758992053866</v>
       </c>
       <c r="F9">
-        <v>0.8029076055890392</v>
+        <v>0.8046708665762504</v>
       </c>
       <c r="G9">
-        <v>0.9600094535782364</v>
+        <v>0.98336390185164</v>
       </c>
     </row>
     <row r="10">
@@ -1180,19 +1181,19 @@
         </is>
       </c>
       <c r="C10">
-        <v>1.463910292077418</v>
+        <v>3.155928332306659</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>11.55604772748408</v>
+        <v>12.5240851518328</v>
       </c>
       <c r="F10">
-        <v>0.1698838355518098</v>
+        <v>0.007899642622595907</v>
       </c>
       <c r="G10">
-        <v>0.3640367904681638</v>
+        <v>0.02369892786778772</v>
       </c>
     </row>
     <row r="11">
@@ -1207,19 +1208,19 @@
         </is>
       </c>
       <c r="C11">
-        <v>7.270438241015258</v>
+        <v>1.936318992284431</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1.000004409932595</v>
+        <v>1.00000517278386</v>
       </c>
       <c r="F11">
-        <v>0.08701609480820602</v>
+        <v>0.3034858176971905</v>
       </c>
       <c r="G11">
-        <v>0.3068871524944256</v>
+        <v>0.5690359081822322</v>
       </c>
     </row>
     <row r="12">
@@ -1234,19 +1235,19 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.2086187641708929</v>
+        <v>0.1865924181457022</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1.000008188624016</v>
+        <v>1.000009488474191</v>
       </c>
       <c r="F12">
-        <v>0.8690668773105277</v>
+        <v>0.8825618621400841</v>
       </c>
       <c r="G12">
-        <v>0.9600094535782364</v>
+        <v>0.98336390185164</v>
       </c>
     </row>
     <row r="13">
@@ -1261,19 +1262,19 @@
         </is>
       </c>
       <c r="C13">
-        <v>1.699688125702346</v>
+        <v>1.488219024285826</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>9.17764130232702</v>
+        <v>9.539346128281155</v>
       </c>
       <c r="F13">
-        <v>0.1227548609977702</v>
+        <v>0.1689863212889058</v>
       </c>
       <c r="G13">
-        <v>0.3068871524944256</v>
+        <v>0.3621135456190838</v>
       </c>
     </row>
     <row r="14">
@@ -1288,19 +1289,19 @@
         </is>
       </c>
       <c r="C14">
-        <v>0.1460392110547658</v>
+        <v>0.309567931083228</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1.834932572983317</v>
+        <v>1.840522572537709</v>
       </c>
       <c r="F14">
-        <v>0.8983350813025558</v>
+        <v>0.7883838335059444</v>
       </c>
       <c r="G14">
-        <v>0.9600094535782364</v>
+        <v>0.98336390185164</v>
       </c>
     </row>
     <row r="15">
@@ -1315,19 +1316,19 @@
         </is>
       </c>
       <c r="C15">
-        <v>0.5327596864735483</v>
+        <v>1.367701705324735</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>1.349047713355914</v>
+        <v>1.28639194939222</v>
       </c>
       <c r="F15">
-        <v>0.6686092200112963</v>
+        <v>0.362444462914999</v>
       </c>
       <c r="G15">
-        <v>0.9600094535782364</v>
+        <v>0.6040741048583317</v>
       </c>
     </row>
     <row r="16">
@@ -1342,19 +1343,19 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.05782218187838763</v>
+        <v>0.05688635245826114</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1.680946341118913</v>
+        <v>1.547872764138074</v>
       </c>
       <c r="F16">
-        <v>0.9600094535782364</v>
+        <v>0.9610947947159141</v>
       </c>
       <c r="G16">
-        <v>0.9600094535782364</v>
+        <v>0.98336390185164</v>
       </c>
     </row>
     <row r="17">
@@ -1369,19 +1370,19 @@
         </is>
       </c>
       <c r="C17">
-        <v>8.159022168185942</v>
+        <v>0.3838606145568483</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>35.53955441607287</v>
+        <v>35.69552461908432</v>
       </c>
       <c r="F17">
-        <v>1.163089618016663e-09</v>
+        <v>0.7033588198889126</v>
       </c>
       <c r="G17">
-        <v>6.97853770809998e-09</v>
+        <v>0.7033588198889126</v>
       </c>
     </row>
     <row r="18">
@@ -1396,19 +1397,19 @@
         </is>
       </c>
       <c r="C18">
-        <v>3.266300946623589</v>
+        <v>1.630097590532166</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>1.000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0.1891369020769736</v>
+        <v>0.3503051007771155</v>
       </c>
       <c r="G18">
-        <v>0.3782738041539472</v>
+        <v>0.5254576511656732</v>
       </c>
     </row>
     <row r="19">
@@ -1423,19 +1424,19 @@
         </is>
       </c>
       <c r="C19">
-        <v>3.447438517521533</v>
+        <v>1.499175741530596</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>4.789509791339096</v>
+        <v>4.359205059832481</v>
       </c>
       <c r="F19">
-        <v>0.01959016219962199</v>
+        <v>0.2024454607297748</v>
       </c>
       <c r="G19">
-        <v>0.05877048659886598</v>
+        <v>0.5254576511656732</v>
       </c>
     </row>
     <row r="20">
@@ -1450,19 +1451,19 @@
         </is>
       </c>
       <c r="C20">
-        <v>1.444922096461102</v>
+        <v>1.674347639661599</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1.043251727552051</v>
+        <v>1.039284206784907</v>
       </c>
       <c r="F20">
-        <v>0.3782395317895865</v>
+        <v>0.3357635555885418</v>
       </c>
       <c r="G20">
-        <v>0.4538874381475038</v>
+        <v>0.5254576511656732</v>
       </c>
     </row>
     <row r="21">
@@ -1477,19 +1478,19 @@
         </is>
       </c>
       <c r="C21">
-        <v>1.056254014633016</v>
+        <v>1.528063534952901</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>5.526461059426611</v>
+        <v>5.256919591404019</v>
       </c>
       <c r="F21">
-        <v>0.3348224817514061</v>
+        <v>0.1842160499475272</v>
       </c>
       <c r="G21">
-        <v>0.4538874381475038</v>
+        <v>0.5254576511656732</v>
       </c>
     </row>
     <row r="22">
@@ -1504,19 +1505,234 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.5114466235943044</v>
+        <v>0.7974327813315768</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1.628291019541396</v>
+        <v>1.420021419896588</v>
       </c>
       <c r="F22">
-        <v>0.6698096821169367</v>
+        <v>0.5366515439152819</v>
       </c>
       <c r="G22">
-        <v>0.6698096821169367</v>
+        <v>0.6439818526983383</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>outcome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>moderator_design</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>n_effect_sizes</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>k_studies</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cross-sectional</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>732</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Experimental (non-randomized)</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Longitudinal</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>65</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Experimental (RCT)</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Cross-lagged</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cross-sectional</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>395</v>
+      </c>
+      <c r="D7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Experimental (non-randomized)</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Longitudinal</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Cross-lagged</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Experimental (non-randomized</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>